<commit_message>
default value by type
</commit_message>
<xml_diff>
--- a/Docs/ExampleData.xlsx
+++ b/Docs/ExampleData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,10 +135,6 @@
   </si>
   <si>
     <t>BS003</t>
-  </si>
-  <si>
-    <t>厉鬼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -527,7 +523,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -724,9 +720,7 @@
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
add mutiple sheet export
</commit_message>
<xml_diff>
--- a/Docs/ExampleData.xlsx
+++ b/Docs/ExampleData.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="NPC" sheetId="1" r:id="rId1"/>
+    <sheet name="Item" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,6 +134,30 @@
   </si>
   <si>
     <t>BS003</t>
+  </si>
+  <si>
+    <t>WP001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WP002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>倚天剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>屠龙刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICON01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICON02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -522,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -758,25 +781,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add Date Time Format string
</commit_message>
<xml_diff>
--- a/Docs/ExampleData.xlsx
+++ b/Docs/ExampleData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="NPC" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,46 +57,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ActPoints</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>战力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ActSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>身法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>命中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dodge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>闪避</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Critical</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>暴击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AssetName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -157,6 +117,18 @@
   </si>
   <si>
     <t>ICON02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DateTest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -230,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -239,6 +211,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -543,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -556,15 +535,11 @@
     <col min="4" max="4" width="6.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="9.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="1"/>
-    <col min="10" max="10" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="10.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -572,7 +547,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>5</v>
@@ -583,31 +558,19 @@
       <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
@@ -618,23 +581,11 @@
       <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -642,10 +593,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>7</v>
@@ -653,31 +604,19 @@
       <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2">
         <v>100</v>
@@ -688,31 +627,19 @@
       <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="2">
-        <v>5</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="I4" s="2">
-        <v>8</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G4" s="5">
+        <v>35800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2">
         <v>352</v>
@@ -723,29 +650,17 @@
       <c r="F5" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="2">
-        <v>32</v>
-      </c>
-      <c r="H5" s="2">
-        <v>4</v>
-      </c>
-      <c r="I5" s="2">
-        <v>3</v>
-      </c>
-      <c r="J5" s="2">
-        <v>4</v>
-      </c>
-      <c r="K5" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G5" s="5">
+        <v>35462</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2">
         <v>332</v>
@@ -756,26 +671,14 @@
       <c r="F6" s="2">
         <v>44</v>
       </c>
-      <c r="G6" s="2">
-        <v>432</v>
-      </c>
-      <c r="H6" s="2">
-        <v>4</v>
-      </c>
-      <c r="I6" s="2">
-        <v>3</v>
-      </c>
-      <c r="J6" s="2">
-        <v>4</v>
-      </c>
-      <c r="K6" s="2">
-        <v>2</v>
+      <c r="G6" s="5">
+        <v>35131</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -783,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -800,18 +703,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -822,29 +725,29 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exclude sheet and column with prefix
</commit_message>
<xml_diff>
--- a/Docs/ExampleData.xlsx
+++ b/Docs/ExampleData.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NPC" sheetId="1" r:id="rId1"/>
     <sheet name="Item" sheetId="2" r:id="rId2"/>
+    <sheet name="#Item" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,6 +130,26 @@
   </si>
   <si>
     <t>测试日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#TestExclude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试过滤列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hello</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试使用前缀过滤掉表单</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -136,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +186,15 @@
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -202,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -218,6 +248,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -522,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -536,10 +569,11 @@
     <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="9.25" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="8" max="8" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -561,8 +595,11 @@
       <c r="G1" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -584,8 +621,11 @@
       <c r="G2" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -607,8 +647,11 @@
       <c r="G3" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -630,8 +673,11 @@
       <c r="G4" s="5">
         <v>35800</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -653,8 +699,11 @@
       <c r="G5" s="5">
         <v>35462</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -673,6 +722,9 @@
       </c>
       <c r="G6" s="5">
         <v>35131</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -754,4 +806,89 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
convert json in cell
</commit_message>
<xml_diff>
--- a/Docs/ExampleData.xlsx
+++ b/Docs/ExampleData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="NPC" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,10 +133,42 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>hello</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试使用前缀过滤掉表单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>["player","enemy"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">     ["player","enemy"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  ["bad array","error"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"player":"enemy"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>#TestExclude</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>TestJsonArray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestJsonObject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -145,11 +177,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>hello</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试使用前缀过滤掉表单</t>
+    <t>测试单元格内的Json数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试单元格内的Json对象</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -555,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -569,11 +601,12 @@
     <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="9.25" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col min="8" max="8" width="14.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="24.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -595,11 +628,17 @@
       <c r="G1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -621,11 +660,17 @@
       <c r="G2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -647,11 +692,17 @@
       <c r="G3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -673,11 +724,17 @@
       <c r="G4" s="5">
         <v>35800</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -699,11 +756,17 @@
       <c r="G5" s="5">
         <v>35462</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J5" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -723,8 +786,14 @@
       <c r="G6" s="5">
         <v>35131</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>32</v>
+      <c r="H6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -812,7 +881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -878,7 +947,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>

</xml_diff>

<commit_message>
test number json array
</commit_message>
<xml_diff>
--- a/Docs/ExampleData.xlsx
+++ b/Docs/ExampleData.xlsx
@@ -145,10 +145,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">     ["player","enemy"]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">  ["bad array","error"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -182,6 +178,10 @@
   </si>
   <si>
     <t>测试单元格内的Json对象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">     [22,33,666]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -590,7 +590,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -629,13 +629,13 @@
         <v>26</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -664,10 +664,10 @@
         <v>13</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -693,13 +693,13 @@
         <v>28</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -731,7 +731,7 @@
         <v>31</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -760,10 +760,10 @@
         <v>29</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -790,10 +790,10 @@
         <v>29</v>
       </c>
       <c r="I6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>